<commit_message>
merged record data with bls mapping data
</commit_message>
<xml_diff>
--- a/assets/bls_cpsaat39_2011_to_2015.xlsx
+++ b/assets/bls_cpsaat39_2011_to_2015.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasw\Documents\UMich\MADS\Courses\SIADS - 593 Milestone 1\Project\Project\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69006D24-5A5F-4E8A-94C6-D400476BD66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15649A1D-8777-4551-BB09-C8D6C86F97F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6760" yWindow="3080" windowWidth="22810" windowHeight="16320" xr2:uid="{7687CDC2-136B-4566-9610-BFBEE6673C5F}"/>
+    <workbookView xWindow="39770" yWindow="6380" windowWidth="19420" windowHeight="16320" xr2:uid="{7687CDC2-136B-4566-9610-BFBEE6673C5F}"/>
   </bookViews>
   <sheets>
     <sheet name="level_mapping_l0" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="2012" sheetId="5" r:id="rId5"/>
     <sheet name="2011" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">level_mapping_l0!$A$1:$F$538</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6074" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6086" uniqueCount="578">
   <si>
     <t>occupation</t>
   </si>
@@ -1770,6 +1773,12 @@
   <si>
     <t>Computer and mathematical occupations</t>
   </si>
+  <si>
+    <t>Undeclared</t>
+  </si>
+  <si>
+    <t>Unclassified</t>
+  </si>
 </sst>
 </file>
 
@@ -2170,11 +2179,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7FAC6B-CBA4-46FF-BD1B-A77A530AFFE3}">
-  <dimension ref="A1:F536"/>
+  <dimension ref="A1:F538"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C540" sqref="C540"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="45.26953125" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" customWidth="1"/>
+    <col min="4" max="4" width="32.54296875" customWidth="1"/>
+    <col min="5" max="5" width="50.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -3370,7 +3387,7 @@
         <v>70</v>
       </c>
       <c r="E60" t="s">
-        <v>70</v>
+        <v>575</v>
       </c>
       <c r="F60" t="s">
         <v>69</v>
@@ -3390,7 +3407,7 @@
         <v>70</v>
       </c>
       <c r="E61" t="s">
-        <v>70</v>
+        <v>575</v>
       </c>
       <c r="F61" t="s">
         <v>71</v>
@@ -3430,7 +3447,7 @@
         <v>70</v>
       </c>
       <c r="E63" t="s">
-        <v>70</v>
+        <v>575</v>
       </c>
       <c r="F63" t="s">
         <v>73</v>
@@ -3490,7 +3507,7 @@
         <v>70</v>
       </c>
       <c r="E66" t="s">
-        <v>70</v>
+        <v>575</v>
       </c>
       <c r="F66" t="s">
         <v>76</v>
@@ -3530,7 +3547,7 @@
         <v>70</v>
       </c>
       <c r="E68" t="s">
-        <v>70</v>
+        <v>575</v>
       </c>
       <c r="F68" t="s">
         <v>78</v>
@@ -3550,7 +3567,7 @@
         <v>70</v>
       </c>
       <c r="E69" t="s">
-        <v>70</v>
+        <v>575</v>
       </c>
       <c r="F69" t="s">
         <v>79</v>
@@ -3570,7 +3587,7 @@
         <v>70</v>
       </c>
       <c r="E70" t="s">
-        <v>70</v>
+        <v>575</v>
       </c>
       <c r="F70" t="s">
         <v>80</v>
@@ -8624,13 +8641,13 @@
         <v>7</v>
       </c>
       <c r="C323" t="s">
-        <v>288</v>
+        <v>8</v>
       </c>
       <c r="D323" t="s">
-        <v>308</v>
+        <v>70</v>
       </c>
       <c r="E323" t="s">
-        <v>308</v>
+        <v>575</v>
       </c>
       <c r="F323" t="s">
         <v>349</v>
@@ -10804,13 +10821,13 @@
         <v>7</v>
       </c>
       <c r="C432" t="s">
-        <v>451</v>
+        <v>8</v>
       </c>
       <c r="D432" t="s">
-        <v>452</v>
+        <v>70</v>
       </c>
       <c r="E432" t="s">
-        <v>452</v>
+        <v>575</v>
       </c>
       <c r="F432" t="s">
         <v>464</v>
@@ -12894,6 +12911,46 @@
       </c>
       <c r="F536" t="s">
         <v>569</v>
+      </c>
+    </row>
+    <row r="537" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A537" t="s">
+        <v>576</v>
+      </c>
+      <c r="B537" t="s">
+        <v>7</v>
+      </c>
+      <c r="C537" t="s">
+        <v>576</v>
+      </c>
+      <c r="D537" t="s">
+        <v>576</v>
+      </c>
+      <c r="E537" t="s">
+        <v>576</v>
+      </c>
+      <c r="F537" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="538" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A538" t="s">
+        <v>577</v>
+      </c>
+      <c r="B538" t="s">
+        <v>7</v>
+      </c>
+      <c r="C538" t="s">
+        <v>577</v>
+      </c>
+      <c r="D538" t="s">
+        <v>577</v>
+      </c>
+      <c r="E538" t="s">
+        <v>577</v>
+      </c>
+      <c r="F538" t="s">
+        <v>577</v>
       </c>
     </row>
   </sheetData>
@@ -13815,7 +13872,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
         <v>44</v>
       </c>
@@ -15149,7 +15206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A98" s="6" t="s">
         <v>101</v>
       </c>
@@ -15839,7 +15896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A128" s="6" t="s">
         <v>131</v>
       </c>
@@ -16667,7 +16724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A164" s="6" t="s">
         <v>167</v>
       </c>
@@ -16851,7 +16908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A172" s="6" t="s">
         <v>175</v>
       </c>
@@ -16897,7 +16954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A174" s="6" t="s">
         <v>177</v>
       </c>
@@ -18438,7 +18495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A241" s="5" t="s">
         <v>244</v>
       </c>
@@ -18507,7 +18564,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A244" s="5" t="s">
         <v>247</v>
       </c>
@@ -18599,7 +18656,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A248" s="5" t="s">
         <v>251</v>
       </c>
@@ -18622,7 +18679,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A249" s="5" t="s">
         <v>252</v>
       </c>
@@ -18829,7 +18886,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A258" s="5" t="s">
         <v>261</v>
       </c>
@@ -19128,7 +19185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A271" s="5" t="s">
         <v>274</v>
       </c>
@@ -19657,7 +19714,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A294" s="5" t="s">
         <v>297</v>
       </c>
@@ -19841,7 +19898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A302" s="5" t="s">
         <v>305</v>
       </c>
@@ -19910,7 +19967,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A305" s="5" t="s">
         <v>307</v>
       </c>
@@ -20485,7 +20542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A330" s="5" t="s">
         <v>333</v>
       </c>
@@ -20531,7 +20588,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="332" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A332" s="5" t="s">
         <v>335</v>
       </c>
@@ -20715,7 +20772,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="340" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A340" s="5" t="s">
         <v>343</v>
       </c>
@@ -20807,7 +20864,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A344" s="5" t="s">
         <v>347</v>
       </c>
@@ -20968,7 +21025,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A351" s="5" t="s">
         <v>354</v>
       </c>
@@ -21106,7 +21163,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="357" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A357" s="1" t="s">
         <v>361</v>
       </c>
@@ -21152,7 +21209,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="359" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A359" s="5" t="s">
         <v>360</v>
       </c>
@@ -21382,7 +21439,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A369" s="5" t="s">
         <v>371</v>
       </c>
@@ -21589,7 +21646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A378" s="5" t="s">
         <v>381</v>
       </c>
@@ -22118,7 +22175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A401" s="5" t="s">
         <v>404</v>
       </c>
@@ -22371,7 +22428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A412" s="5" t="s">
         <v>415</v>
       </c>
@@ -22440,7 +22497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A415" s="5" t="s">
         <v>418</v>
       </c>
@@ -22486,7 +22543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A417" s="5" t="s">
         <v>420</v>
       </c>
@@ -22509,7 +22566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A418" s="5" t="s">
         <v>421</v>
       </c>
@@ -22670,7 +22727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A425" s="5" t="s">
         <v>428</v>
       </c>
@@ -22716,7 +22773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A427" s="5" t="s">
         <v>430</v>
       </c>
@@ -22762,7 +22819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A429" s="5" t="s">
         <v>432</v>
       </c>
@@ -22992,7 +23049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A439" s="5" t="s">
         <v>442</v>
       </c>
@@ -23245,7 +23302,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="450" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A450" s="5" t="s">
         <v>453</v>
       </c>
@@ -23383,7 +23440,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="456" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="456" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A456" s="5" t="s">
         <v>459</v>
       </c>
@@ -23406,7 +23463,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="457" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="457" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A457" s="5" t="s">
         <v>460</v>
       </c>
@@ -23521,7 +23578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="462" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="462" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A462" s="5" t="s">
         <v>465</v>
       </c>
@@ -23544,7 +23601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="463" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A463" s="5" t="s">
         <v>466</v>
       </c>
@@ -23567,7 +23624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="464" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="464" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A464" s="5" t="s">
         <v>467</v>
       </c>
@@ -23613,7 +23670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="466" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="466" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A466" s="5" t="s">
         <v>469</v>
       </c>
@@ -23659,7 +23716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="468" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="468" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A468" s="5" t="s">
         <v>471</v>
       </c>
@@ -23682,7 +23739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="469" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="469" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A469" s="5" t="s">
         <v>472</v>
       </c>
@@ -23774,7 +23831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="473" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="473" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A473" s="5" t="s">
         <v>476</v>
       </c>
@@ -23797,7 +23854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="474" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="474" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A474" s="5" t="s">
         <v>477</v>
       </c>
@@ -23866,7 +23923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="477" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="477" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A477" s="5" t="s">
         <v>480</v>
       </c>
@@ -23912,7 +23969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="479" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="479" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A479" s="5" t="s">
         <v>482</v>
       </c>
@@ -24234,7 +24291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="493" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="493" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A493" s="5" t="s">
         <v>496</v>
       </c>
@@ -24257,7 +24314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="494" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="494" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A494" s="5" t="s">
         <v>497</v>
       </c>
@@ -24464,7 +24521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="503" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="503" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A503" s="5" t="s">
         <v>506</v>
       </c>
@@ -24556,7 +24613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="507" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="507" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A507" s="5" t="s">
         <v>510</v>
       </c>
@@ -24602,7 +24659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="509" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="509" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A509" s="5" t="s">
         <v>512</v>
       </c>
@@ -24671,7 +24728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="512" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="512" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A512" s="5" t="s">
         <v>515</v>
       </c>
@@ -24832,7 +24889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="519" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="519" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A519" s="5" t="s">
         <v>522</v>
       </c>
@@ -24901,7 +24958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="522" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="522" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A522" s="5" t="s">
         <v>525</v>
       </c>
@@ -25200,7 +25257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="535" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="535" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A535" s="5" t="s">
         <v>538</v>
       </c>

</xml_diff>